<commit_message>
Made the benchmark Chart
</commit_message>
<xml_diff>
--- a/FlairResearch/Flair Reseach Results.xlsx
+++ b/FlairResearch/Flair Reseach Results.xlsx
@@ -774,7 +774,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2545,11 +2545,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="63697749"/>
-        <c:axId val="38436272"/>
+        <c:axId val="938879"/>
+        <c:axId val="5569215"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63697749"/>
+        <c:axId val="938879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2609,14 +2609,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38436272"/>
+        <c:crossAx val="5569215"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38436272"/>
+        <c:axId val="5569215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,7 +2655,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63697749"/>
+        <c:crossAx val="938879"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2706,7 +2706,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3278,11 +3278,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="66434342"/>
-        <c:axId val="67454003"/>
+        <c:axId val="57827620"/>
+        <c:axId val="1228076"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66434342"/>
+        <c:axId val="57827620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3314,14 +3314,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67454003"/>
+        <c:crossAx val="1228076"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67454003"/>
+        <c:axId val="1228076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,7 +3360,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66434342"/>
+        <c:crossAx val="57827620"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5053,8 +5053,8 @@
   </sheetPr>
   <dimension ref="A3:V54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8181,7 +8181,7 @@
   <dimension ref="A3:T34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10009,8 +10009,8 @@
   </sheetPr>
   <dimension ref="A3:V54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V27" activeCellId="0" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13059,8 +13059,8 @@
   </sheetPr>
   <dimension ref="A3:V54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16115,8 +16115,8 @@
   </sheetPr>
   <dimension ref="B3:AF54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U3" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA15" activeCellId="0" sqref="AA15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB17" activeCellId="0" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>